<commit_message>
Observations + Profiles: added new figures; changes table in TeX
</commit_message>
<xml_diff>
--- a/Observations/OMEXDIA/4_PE138_99-17_4298m.xlsx
+++ b/Observations/OMEXDIA/4_PE138_99-17_4298m.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ads.bris.ac.uk\filestore\MyFiles\Students\dh12423\Documents\OMEXDIA_database\MyProfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dh12423\Dropbox\5_Benthic_model\OMEXDIA\My_Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="NO3" sheetId="3" r:id="rId4"/>
     <sheet name="NH4" sheetId="1" r:id="rId5"/>
     <sheet name="PO4" sheetId="2" r:id="rId6"/>
-    <sheet name="porosity" sheetId="4" r:id="rId7"/>
-    <sheet name="SO4" sheetId="7" r:id="rId8"/>
-    <sheet name="H2S" sheetId="8" r:id="rId9"/>
-    <sheet name="fluxes" sheetId="9" r:id="rId10"/>
+    <sheet name="DIC" sheetId="11" r:id="rId7"/>
+    <sheet name="porosity" sheetId="4" r:id="rId8"/>
+    <sheet name="SO4" sheetId="7" r:id="rId9"/>
+    <sheet name="H2S" sheetId="8" r:id="rId10"/>
+    <sheet name="fluxes" sheetId="9" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'O2'!$A$1:$K$1</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5603" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5757" uniqueCount="86">
   <si>
     <t>Distance</t>
   </si>
@@ -280,11 +281,32 @@
   <si>
     <t>SSIOISSS</t>
   </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>TCO2CAD2</t>
+  </si>
+  <si>
+    <t>TCO2</t>
+  </si>
+  <si>
+    <t>Total dissolved inorganic carbon (TCO2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +379,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -366,8 +388,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,8 +476,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Corg" xfId="3"/>
     <cellStyle name="Normal_fluxes" xfId="7"/>
@@ -463,6 +498,7 @@
     <cellStyle name="Normal_O2" xfId="6"/>
     <cellStyle name="Normal_PO4" xfId="2"/>
     <cellStyle name="Normal_porosity" xfId="5"/>
+    <cellStyle name="Normal_Sheet2" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -752,6 +788,26 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1222,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>260241</v>
       </c>
@@ -1513,7 +1569,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>260241</v>
       </c>
@@ -1548,7 +1604,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>260241</v>
       </c>
@@ -1583,7 +1639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>260241</v>
       </c>
@@ -1618,7 +1674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>260241</v>
       </c>
@@ -1653,7 +1709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>260241</v>
       </c>
@@ -1688,7 +1744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>260241</v>
       </c>
@@ -1723,7 +1779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>260241</v>
       </c>
@@ -1758,7 +1814,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>260241</v>
       </c>
@@ -1793,7 +1849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>260241</v>
       </c>
@@ -1828,7 +1884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>260241</v>
       </c>
@@ -1863,7 +1919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>260241</v>
       </c>
@@ -1898,7 +1954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>260241</v>
       </c>
@@ -33123,6 +33179,948 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="30">
+        <v>-2</v>
+      </c>
+      <c r="D2" s="32">
+        <v>2308</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H2" s="30">
+        <v>34206</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M2" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N2" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="30">
+        <v>0.125</v>
+      </c>
+      <c r="D3" s="32">
+        <v>2409</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H3" s="30">
+        <v>34184</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M3" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="30">
+        <v>0.375</v>
+      </c>
+      <c r="D4" s="32">
+        <v>2434</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H4" s="30">
+        <v>34185</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M4" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N4" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="30">
+        <v>0.625</v>
+      </c>
+      <c r="D5" s="32">
+        <v>2492</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H5" s="30">
+        <v>34186</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M5" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N5" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="30">
+        <v>0.875</v>
+      </c>
+      <c r="D6" s="32">
+        <v>2536</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H6" s="30">
+        <v>34187</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M6" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N6" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="30">
+        <v>1.25</v>
+      </c>
+      <c r="D7" s="32">
+        <v>2594</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H7" s="30">
+        <v>34188</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M7" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1.75</v>
+      </c>
+      <c r="D8" s="32">
+        <v>2603</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H8" s="30">
+        <v>34189</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M8" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N8" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="30">
+        <v>2.25</v>
+      </c>
+      <c r="D9" s="32">
+        <v>2775</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H9" s="30">
+        <v>34190</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M9" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N9" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="30">
+        <v>2.75</v>
+      </c>
+      <c r="D10" s="32">
+        <v>2877</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H10" s="30">
+        <v>34127</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M10" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N10" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="30">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="32">
+        <v>2945</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H11" s="30">
+        <v>34128</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M11" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N11" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="30">
+        <v>4.5</v>
+      </c>
+      <c r="D12" s="32">
+        <v>3106</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H12" s="30">
+        <v>34129</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M12" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N12" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="30">
+        <v>5.5</v>
+      </c>
+      <c r="D13" s="32">
+        <v>3152</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H13" s="30">
+        <v>34130</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M13" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N13" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="30">
+        <v>6.5</v>
+      </c>
+      <c r="D14" s="32">
+        <v>3193</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H14" s="30">
+        <v>34131</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L14" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M14" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N14" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="30">
+        <v>8</v>
+      </c>
+      <c r="D15" s="32">
+        <v>3197</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H15" s="30">
+        <v>34132</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M15" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N15" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="30">
+        <v>10</v>
+      </c>
+      <c r="D16" s="32">
+        <v>3307</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H16" s="30">
+        <v>34133</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M16" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N16" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="30">
+        <v>12</v>
+      </c>
+      <c r="D17" s="32">
+        <v>3300</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H17" s="30">
+        <v>34134</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M17" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N17" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="30">
+        <v>14</v>
+      </c>
+      <c r="D18" s="32">
+        <v>3220</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H18" s="30">
+        <v>34135</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L18" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M18" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N18" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="30">
+        <v>16</v>
+      </c>
+      <c r="D19" s="32">
+        <v>3280</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H19" s="30">
+        <v>34124</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M19" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N19" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="30">
+        <v>18</v>
+      </c>
+      <c r="D20" s="32">
+        <v>3280</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H20" s="30">
+        <v>34125</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M20" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N20" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="30">
+        <v>260241</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="30">
+        <v>20</v>
+      </c>
+      <c r="D21" s="32">
+        <v>3470</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="30">
+        <v>4280</v>
+      </c>
+      <c r="H21" s="30">
+        <v>34126</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L21" s="30">
+        <v>39.579329999999999</v>
+      </c>
+      <c r="M21" s="30">
+        <v>-10.275169999999999</v>
+      </c>
+      <c r="N21" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33741,26 +34739,6 @@
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="Q2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33779,7 +34757,7 @@
   <sheetData>
     <row r="2" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>